<commit_message>
fixed: change_page, hasil_tes, progress, scoring, sidebars
</commit_message>
<xml_diff>
--- a/misc/databasestudentmodel.xlsx
+++ b/misc/databasestudentmodel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Tesis\Program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\My-Projects\pasti\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="621"/>
+    <workbookView xWindow="0" yWindow="1380" windowWidth="20490" windowHeight="7155" tabRatio="621" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Siswa" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>jumlah_tes</t>
   </si>
   <si>
-    <t>jumah_pertanyaan</t>
-  </si>
-  <si>
     <t>Q15</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>Jumlah</t>
+  </si>
+  <si>
+    <t>jumlah_pertanyaan</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -526,10 +526,15 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -555,10 +560,16 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -627,11 +638,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -644,7 +661,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
@@ -673,52 +690,52 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>